<commit_message>
adding the solution to the container_with_most_water problem.
</commit_message>
<xml_diff>
--- a/key_notes.xlsx
+++ b/key_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ketanpatil/Desktop/codepath-summer-24/blind75/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ketanpatil/Desktop/codepath-summer-24/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4ABCBB-26D6-3449-BB90-3F3F7EF857ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C264BE3-9BE0-A24B-AB0F-62D7BCF31DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{83CFC674-736D-B547-BBE8-BA3EBD5788F7}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{83CFC674-736D-B547-BBE8-BA3EBD5788F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>BLIND 75</t>
   </si>
@@ -111,6 +111,94 @@
     <t>1. Dict to store key as letter and value as its frequency in the string.
 2. Maintain two such dicts for two strings
 3. Compare the two dict, if equal its an anagram</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Hashmap</t>
+  </si>
+  <si>
+    <t>Hashmap (Dictionary)</t>
+  </si>
+  <si>
+    <t>1. Store and retrieve elements in O(1) time in a hashmap
+2. know the time complexities of insert/find/delete operations in hashmap which is O(1)
+3. consider edge cases such as empty input array, no possible matches, multiple pairs with same value as target
+4. space complexity tradeoff with time: introduce additional space for the new hashmap</t>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
+  </si>
+  <si>
+    <t>Hashmap (Dictionary), Tuple</t>
+  </si>
+  <si>
+    <t>1. Use character frequency count as a unique key for our hashmap.
+2. these character counts will be grouped as keys in the form of a tuple cause keys in the hashmap cannot be a list.
+3. anagram will belong to a common tuple pattern and will be appended in the list which is the value of our key.
+4. we will use defaultdict() from the collections class since we wanna keep the default value as an empty list if not anagram groups are found
+5.make sure to return the result as a list to get a grouped list of anagram lists
+6. time complexity: n-number of strings as input, k-len of string so, O(n*k)
+7. space complexity: O(n*k) to store the result and character counts</t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>Frequency Count, Bucket Sort</t>
+  </si>
+  <si>
+    <t>Hashmap (Dictionary), List</t>
+  </si>
+  <si>
+    <t>1. Edge Case Handling:
+    - Empty List: Always check if the input list is empty or if k is 0, as these require immediate returns of an empty list.
+   - Single Element: Consider what happens when the list contains only one element, or all elements are the same.
+2. Efficiency Considerations:
+    - Using a dictionary for counting is much more efficient than repeatedly scanning the array.
+    - Leveraging the properties of arrays (where index access is O(1)) for bucketing can drastically reduce the time needed for organizing and sorting data based on frequency.
+3. Sorting Optimization:
+    - You do not need to sort the entire list of elements; you only need the top k elements. This is where bucket sorting (using the array of lists) shines, as it inherently sorts elements by frequency due to the structure of the storage.
+4. Use of Python Built-ins:
+    - Utilize Python’s collections.Counter for counting elements as it is optimized for this task and reduces the code complexity.
+    - Python’s list comprehensions and slicing can simplify and speed up the process of collecting the top kk elements once they are bucketed.</t>
+  </si>
+  <si>
+    <t>Decode String</t>
+  </si>
+  <si>
+    <t>Two Sum Two</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Hashmap (Dictionary - Counter from Collections)</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Two Pointers ( Two Sum Two )</t>
+  </si>
+  <si>
+    <t>Three Sum</t>
+  </si>
+  <si>
+    <t>1. Sorting: Start by sorting the array to simplify finding and skipping duplicates
+2. Two pointer method: For each element, use two pointers (left and right) to find pairs that sum up to the negative fixed element.
+3. Avoid Duplicates: Skip duplicate elements by checking the current element agianst the previous one to avoid redundant triplets
+4. Complexity: The approach typically results in sorting (O(nlogn)) and O(n^2), so overall O(n^2).</t>
+  </si>
+  <si>
+    <t>1. Parsing: Traverse the stirng char by char
+2. Stacks: Push numbers and substrings onto their respective stacks when encountering '['. Pop and build the decoded string when encountering ']'
+3. Reconstruction: Concatenate the repeated substrings using the numbers from the stack.
+4. Typically O(n) where n is the length of the string, due to single pass parsing and stack operations</t>
   </si>
 </sst>
 </file>
@@ -530,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610DAE46-8EB7-2941-917E-C9656203289B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,7 +629,7 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="1" customWidth="1"/>
-    <col min="5" max="5" width="54" style="5" customWidth="1"/>
+    <col min="5" max="5" width="86.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -563,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -589,6 +677,101 @@
       </c>
       <c r="E4" s="4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="356" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding solution to the longest substring without repeating characters problem
</commit_message>
<xml_diff>
--- a/key_notes.xlsx
+++ b/key_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ketanpatil/Desktop/codepath-summer-24/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C264BE3-9BE0-A24B-AB0F-62D7BCF31DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E544F6C0-CC0B-BE42-85FB-7449FCB30BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{83CFC674-736D-B547-BBE8-BA3EBD5788F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>BLIND 75</t>
   </si>
@@ -199,6 +199,47 @@
 2. Stacks: Push numbers and substrings onto their respective stacks when encountering '['. Pop and build the decoded string when encountering ']'
 3. Reconstruction: Concatenate the repeated substrings using the numbers from the stack.
 4. Typically O(n) where n is the length of the string, due to single pass parsing and stack operations</t>
+  </si>
+  <si>
+    <t>Container with most water</t>
+  </si>
+  <si>
+    <t>1. Initialize two pointers at the two ends of the array and calculate the area formed by the lines they point to
+2. Move the pointer pointing to the shorter line inward to potentially find a taller line and a larger area
+3. The two pointer approach makes sure an O(n) time complexity by making a single pass through the array</t>
+  </si>
+  <si>
+    <t>1. Counting: Traverse both strings and count character occurences 
+2. Comparison: Compare the character count for both strings
+3. Alternatively sort both strings and do a direct comparison
+4. Counting is O(n), sorting is O(n*logn)</t>
+  </si>
+  <si>
+    <t>1. Pointer initialization: Initialize two pointers at the beiginning and end of the array.
+2. Pointer movement: Move the left pointer inwards or the right pointer inwards based on the sum comparison with the target
+3. Edge cases: handle cases where array has fewer than two elements 
+4. O(n) due to a single pass with two pointers</t>
+  </si>
+  <si>
+    <t>Best time to buy and sell stock</t>
+  </si>
+  <si>
+    <t>Note: try this problem out with greedy approach the next time you see this
+1. Learn about greedy algorithm.</t>
+  </si>
+  <si>
+    <t>Longest substring without repeating characters</t>
+  </si>
+  <si>
+    <t>Hashmap or Set</t>
+  </si>
+  <si>
+    <t>1. Use sliding window technique to maintain a substring with unique chars.
+2. window is defined by two pointers: start and end / left and right
+3. as we traverse based on conditions we adjust the window size dynamically
+4. we have the hashmap to store key ( char ) and value ( index position of that char )
+5. if a repeating character is found we move the position of the start pointer next to the last seen index of the repeating char. then update the hashmap with current index of the char
+6. we calculate the current window size : end - start + 1 , and then update the max_len( max len of the substring).</t>
   </si>
 </sst>
 </file>
@@ -618,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610DAE46-8EB7-2941-917E-C9656203289B}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,7 +776,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -745,11 +786,11 @@
       <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
@@ -758,6 +799,9 @@
       </c>
       <c r="D10" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.2">
@@ -772,6 +816,48 @@
       </c>
       <c r="E11" s="4" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding solution to the longest repeating character replacement problem
</commit_message>
<xml_diff>
--- a/key_notes.xlsx
+++ b/key_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ketanpatil/Desktop/codepath-summer-24/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E544F6C0-CC0B-BE42-85FB-7449FCB30BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C540D4-D453-1847-BD7E-A52BA9E50DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{83CFC674-736D-B547-BBE8-BA3EBD5788F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>BLIND 75</t>
   </si>
@@ -240,6 +240,9 @@
 4. we have the hashmap to store key ( char ) and value ( index position of that char )
 5. if a repeating character is found we move the position of the start pointer next to the last seen index of the repeating char. then update the hashmap with current index of the char
 6. we calculate the current window size : end - start + 1 , and then update the max_len( max len of the substring).</t>
+  </si>
+  <si>
+    <t>Longest repeating character replacement</t>
   </si>
 </sst>
 </file>
@@ -659,16 +662,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610DAE46-8EB7-2941-917E-C9656203289B}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="262" zoomScaleNormal="262" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="1" customWidth="1"/>
     <col min="5" max="5" width="86.1640625" style="5" customWidth="1"/>
   </cols>
@@ -860,6 +863,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added solution to the reverse linked list problem
</commit_message>
<xml_diff>
--- a/key_notes.xlsx
+++ b/key_notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ketanpatil/Desktop/codepath-summer-24/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C540D4-D453-1847-BD7E-A52BA9E50DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2496066C-183E-6C4D-BB1D-39EBE5A07D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{83CFC674-736D-B547-BBE8-BA3EBD5788F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>BLIND 75</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Longest repeating character replacement</t>
+  </si>
+  <si>
+    <t>1. current window size - this is typically represented by a formula: (end - start + 1)</t>
   </si>
 </sst>
 </file>
@@ -664,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610DAE46-8EB7-2941-917E-C9656203289B}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="262" zoomScaleNormal="262" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="262" zoomScaleNormal="262" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,6 +870,9 @@
       <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E15" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>